<commit_message>
UPdated functionaled category tree
</commit_message>
<xml_diff>
--- a/downloads/categories.xlsx
+++ b/downloads/categories.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>Категория</t>
   </si>
@@ -20,18 +20,12 @@
     <t>Родитель</t>
   </si>
   <si>
-    <t>Yernaz</t>
+    <t>Электроника</t>
   </si>
   <si>
     <t>—</t>
   </si>
   <si>
-    <t>Nu</t>
-  </si>
-  <si>
-    <t>Электроника</t>
-  </si>
-  <si>
     <t>Телефоны</t>
   </si>
   <si>
@@ -44,22 +38,25 @@
     <t>Samsung</t>
   </si>
   <si>
-    <t>Ноутбуки</t>
-  </si>
-  <si>
-    <t>Asus</t>
-  </si>
-  <si>
-    <t>HP</t>
-  </si>
-  <si>
     <t>Electronics</t>
   </si>
   <si>
-    <t>Ars</t>
-  </si>
-  <si>
-    <t>Beka</t>
+    <t>Yers</t>
+  </si>
+  <si>
+    <t>sdu</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>YersGay</t>
+  </si>
+  <si>
+    <t>Who</t>
   </si>
 </sst>
 </file>
@@ -104,7 +101,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -139,7 +136,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -155,7 +152,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -163,7 +160,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
@@ -171,7 +168,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
@@ -179,7 +176,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10">
@@ -187,7 +184,7 @@
         <v>11</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
@@ -195,7 +192,7 @@
         <v>12</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12">
@@ -211,15 +208,7 @@
         <v>14</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="B14" t="s" s="0">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Text helper util has created
</commit_message>
<xml_diff>
--- a/downloads/categories.xlsx
+++ b/downloads/categories.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>Категория</t>
   </si>
@@ -38,25 +38,13 @@
     <t>Samsung</t>
   </si>
   <si>
-    <t>Electronics</t>
+    <t>Ноутбуки</t>
   </si>
   <si>
-    <t>Yers</t>
+    <t>Asus</t>
   </si>
   <si>
-    <t>sdu</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>YersGay</t>
-  </si>
-  <si>
-    <t>Who</t>
+    <t>HP</t>
   </si>
 </sst>
 </file>
@@ -101,7 +89,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -160,7 +148,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
@@ -168,7 +156,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
@@ -176,39 +164,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s" s="0">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s" s="0">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s" s="0">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s" s="0">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Full Test has completed
</commit_message>
<xml_diff>
--- a/downloads/categories.xlsx
+++ b/downloads/categories.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Категория</t>
   </si>
@@ -20,31 +20,13 @@
     <t>Родитель</t>
   </si>
   <si>
-    <t>Электроника</t>
+    <t>Movies</t>
   </si>
   <si>
     <t>—</t>
   </si>
   <si>
-    <t>Телефоны</t>
-  </si>
-  <si>
-    <t>Смартфоны</t>
-  </si>
-  <si>
-    <t>iPhone</t>
-  </si>
-  <si>
-    <t>Samsung</t>
-  </si>
-  <si>
-    <t>Ноутбуки</t>
-  </si>
-  <si>
-    <t>Asus</t>
-  </si>
-  <si>
-    <t>HP</t>
+    <t>Action</t>
   </si>
 </sst>
 </file>
@@ -89,7 +71,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -119,54 +101,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s" s="0">
-        <v>8</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>